<commit_message>
Added Scripts to create a docker container so it can easily be shared in the future
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg3699892.sharepoint.com/sites/OneForecast/Shared Documents/Projects/Cement Australia/13 Simulation/06 Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_5D13D52ACC30DA92E75E4AE6ADB90931BA360462" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_5D13D52ACC30DA92E75E4AE6ADB90931BA360462" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A37D0002-EDB4-4A04-B478-3D6922E9B947}"/>
   <bookViews>
-    <workbookView xWindow="33870" yWindow="2730" windowWidth="19035" windowHeight="14550" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
@@ -8925,7 +8925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -9246,9 +9246,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -9958,15 +9972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef0ff67e-9087-4832-8b9d-0b53066cc775">
@@ -9975,6 +9980,15 @@
     <TaxCatchAll xmlns="89e87ded-6359-4f8b-890f-4b93e2ce9d62" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10233,20 +10247,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE8FB33B-77C1-497A-8D8D-97EFCEB699BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ADF06DC-4C11-4392-921B-5577076E3FFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="ef0ff67e-9087-4832-8b9d-0b53066cc775"/>
     <ds:schemaRef ds:uri="89e87ded-6359-4f8b-890f-4b93e2ce9d62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE8FB33B-77C1-497A-8D8D-97EFCEB699BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add network map section with download and view functionality
Adds a new section for the network map including a download endpoint in `app.py`, adjusts the layout in `templates/index.html` to accommodate three file sections, and enables input preparation by default in `supply_chain_viz_config.py`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: c872a2a2-cbd7-44c2-9305-5e1447e45d55
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/aDqPeYz
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7617,7 +7617,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7668,7 +7668,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7702,7 +7702,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7719,7 +7719,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7736,7 +7736,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7753,7 +7753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7770,7 +7770,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:44</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7787,7 +7787,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7821,7 +7821,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7838,7 +7838,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7855,7 +7855,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7872,7 +7872,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7906,7 +7906,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7923,7 +7923,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7940,7 +7940,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7957,7 +7957,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7974,7 +7974,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7991,7 +7991,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:33</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8008,7 +8008,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:34</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8025,7 +8025,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:34</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8042,7 +8042,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:34</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8059,7 +8059,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:45</t>
+          <t>2025-12-18 04:38:34</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8076,7 +8076,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:46</t>
+          <t>2025-12-18 04:38:34</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8093,7 +8093,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:46</t>
+          <t>2025-12-18 04:38:35</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8110,7 +8110,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:46</t>
+          <t>2025-12-18 04:38:35</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8127,7 +8127,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:46</t>
+          <t>2025-12-18 04:38:35</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8144,7 +8144,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-18 04:25:47</t>
+          <t>2025-12-18 04:38:35</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">

</xml_diff>

<commit_message>
Add distribution curves to simulation report for variability analysis
Update Network_Map.html to include Plotly charts for visualizing variability drivers.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 20dd0286-6213-47e3-82e5-53e15a8f1bcb
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/aDqPeYz
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7617,7 +7617,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7668,7 +7668,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7702,7 +7702,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7719,7 +7719,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7736,7 +7736,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7753,7 +7753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7770,7 +7770,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7787,7 +7787,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7821,7 +7821,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7838,7 +7838,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7855,7 +7855,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7872,7 +7872,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7906,7 +7906,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7923,7 +7923,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7940,7 +7940,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7957,7 +7957,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7974,7 +7974,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7991,7 +7991,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:33</t>
+          <t>2025-12-18 05:23:05</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8008,7 +8008,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:34</t>
+          <t>2025-12-18 05:23:06</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8025,7 +8025,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:34</t>
+          <t>2025-12-18 05:23:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8042,7 +8042,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:34</t>
+          <t>2025-12-18 05:23:06</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8059,7 +8059,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:34</t>
+          <t>2025-12-18 05:23:06</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8076,7 +8076,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:34</t>
+          <t>2025-12-18 05:23:06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8093,7 +8093,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:35</t>
+          <t>2025-12-18 05:23:07</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8110,7 +8110,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:35</t>
+          <t>2025-12-18 05:23:07</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8127,7 +8127,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:35</t>
+          <t>2025-12-18 05:23:07</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8144,7 +8144,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-18 04:38:35</t>
+          <t>2025-12-18 05:23:07</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">

</xml_diff>

<commit_message>
Improve chart layouts to prevent axis labels from being cut off
Update CSS to ensure plot containers and SVG elements have sufficient overflow and padding, resolving issues with clipped axis labels in the variability report.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 600419d0-4701-4595-8123-66b0d9bfe45a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/C2akjPt
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7617,7 +7617,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7668,7 +7668,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7702,7 +7702,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7719,7 +7719,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7736,7 +7736,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7753,7 +7753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7770,7 +7770,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7787,7 +7787,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7821,7 +7821,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7838,7 +7838,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7855,7 +7855,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7872,7 +7872,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7906,7 +7906,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7923,7 +7923,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7940,7 +7940,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7957,7 +7957,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7974,7 +7974,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7991,7 +7991,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:05</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8008,7 +8008,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:06</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8025,7 +8025,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:06</t>
+          <t>2025-12-18 06:57:15</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8042,7 +8042,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:06</t>
+          <t>2025-12-18 06:57:16</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8059,7 +8059,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:06</t>
+          <t>2025-12-18 06:57:16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8076,7 +8076,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:06</t>
+          <t>2025-12-18 06:57:16</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8093,7 +8093,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:07</t>
+          <t>2025-12-18 06:57:16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8110,7 +8110,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:07</t>
+          <t>2025-12-18 06:57:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8127,7 +8127,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:07</t>
+          <t>2025-12-18 06:57:17</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8144,7 +8144,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-18 05:23:07</t>
+          <t>2025-12-18 06:57:17</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">

</xml_diff>

<commit_message>
Restore header layout and button/link arrangement
Revert header layout changes in `sim_run_report_plot.py` to place the run simulation button and variability link on the same line, separated by a pipe.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 042c3be5-bcaa-412d-a11a-54bd49e15e7f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 0ccb8bda-9225-4449-a453-233ca8a3b9c0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7021497b-e239-4ebb-aabe-96a6d9a99b74/042c3be5-bcaa-412d-a11a-54bd49e15e7f/jT0MXz6
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7617,7 +7617,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7668,7 +7668,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7702,7 +7702,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7719,7 +7719,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7736,7 +7736,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7753,7 +7753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7770,7 +7770,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7787,7 +7787,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7804,7 +7804,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7821,7 +7821,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7838,7 +7838,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7855,7 +7855,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7872,7 +7872,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7906,7 +7906,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7923,7 +7923,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7940,7 +7940,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7957,7 +7957,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7974,7 +7974,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7991,7 +7991,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8008,7 +8008,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8025,7 +8025,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:15</t>
+          <t>2025-12-18 07:57:13</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8042,7 +8042,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:16</t>
+          <t>2025-12-18 07:57:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8059,7 +8059,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:16</t>
+          <t>2025-12-18 07:57:13</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8076,7 +8076,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:16</t>
+          <t>2025-12-18 07:57:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8093,7 +8093,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:16</t>
+          <t>2025-12-18 07:57:13</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8110,7 +8110,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:16</t>
+          <t>2025-12-18 07:57:14</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8127,7 +8127,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:17</t>
+          <t>2025-12-18 07:57:14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8144,7 +8144,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-18 06:57:17</t>
+          <t>2025-12-18 07:57:14</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">

</xml_diff>

<commit_message>
Shipping Review in Progress
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -686,10 +686,6 @@
           <t>GladstoneStoreCL</t>
         </is>
       </c>
-      <c r="S3">
-        <f>IF(ISNA(XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -7298,7 +7294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7566,15 +7562,30 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Osborne</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Osborne</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Port Kembla</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C19" t="n">
         <v>940</v>
       </c>
     </row>
@@ -7617,7 +7628,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7634,7 +7645,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7651,7 +7662,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7668,7 +7679,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7685,7 +7696,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7702,7 +7713,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7719,7 +7730,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7736,7 +7747,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7753,7 +7764,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:05</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7770,7 +7781,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7787,7 +7798,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7804,7 +7815,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7821,7 +7832,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7831,14 +7842,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SHIP_DISTANCES -&gt; SHIP_DISTANCES, rows=17</t>
+          <t>SHIP_DISTANCES -&gt; SHIP_DISTANCES, rows=18</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7855,7 +7866,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7872,7 +7883,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7889,7 +7900,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7906,7 +7917,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7923,7 +7934,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7940,7 +7951,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7957,7 +7968,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7974,7 +7985,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7991,7 +8002,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:06</t>
+          <t>2025-12-20 23:22:07</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8001,14 +8012,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SHIP_DISTANCES rows=17 -&gt; generated_model_inputs.xlsx</t>
+          <t>SHIP_DISTANCES rows=18 -&gt; generated_model_inputs.xlsx</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:07</t>
+          <t>2025-12-20 23:22:08</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8025,7 +8036,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:07</t>
+          <t>2025-12-20 23:22:09</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8042,7 +8053,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:08</t>
+          <t>2025-12-20 23:22:09</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8059,7 +8070,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:08</t>
+          <t>2025-12-20 23:22:10</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8076,7 +8087,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:09</t>
+          <t>2025-12-20 23:22:10</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8093,7 +8104,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:10</t>
+          <t>2025-12-20 23:22:11</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8110,7 +8121,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:10</t>
+          <t>2025-12-20 23:22:11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8127,7 +8138,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:10</t>
+          <t>2025-12-20 23:22:12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8144,7 +8155,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-19 22:42:11</t>
+          <t>2025-12-20 23:22:12</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -8860,7 +8871,7 @@
         <v>3000</v>
       </c>
       <c r="E2" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="F2" t="n">
         <v>500</v>
@@ -9112,7 +9123,7 @@
         <v>3000</v>
       </c>
       <c r="E8" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="F8" t="n">
         <v>500</v>
@@ -9154,7 +9165,7 @@
         <v>3000</v>
       </c>
       <c r="E9" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F9" t="n">
         <v>500</v>
@@ -9196,7 +9207,7 @@
         <v>3000</v>
       </c>
       <c r="E10" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F10" t="n">
         <v>500</v>
@@ -9238,7 +9249,7 @@
         <v>25000</v>
       </c>
       <c r="E11" t="n">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="F11" t="n">
         <v>12500</v>
@@ -9280,7 +9291,7 @@
         <v>120000</v>
       </c>
       <c r="E12" t="n">
-        <v>60000</v>
+        <v>120000</v>
       </c>
       <c r="F12" t="n">
         <v>30000</v>
@@ -9322,7 +9333,7 @@
         <v>14000</v>
       </c>
       <c r="E13" t="n">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="F13" t="n">
         <v>2000</v>
@@ -9490,7 +9501,7 @@
         <v>3000</v>
       </c>
       <c r="E17" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="F17" t="n">
         <v>500</v>
@@ -9522,7 +9533,7 @@
         <v>15000</v>
       </c>
       <c r="E18" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F18" t="n">
         <v>1000</v>
@@ -9564,7 +9575,7 @@
         <v>35000</v>
       </c>
       <c r="E19" t="n">
-        <v>25000</v>
+        <v>35000</v>
       </c>
       <c r="F19" t="n">
         <v>8000</v>
@@ -9606,7 +9617,7 @@
         <v>25000</v>
       </c>
       <c r="E20" t="n">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="F20" t="n">
         <v>5000</v>
@@ -9648,7 +9659,7 @@
         <v>25000</v>
       </c>
       <c r="E21" t="n">
-        <v>18000</v>
+        <v>25000</v>
       </c>
       <c r="F21" t="n">
         <v>2500</v>
@@ -9732,7 +9743,7 @@
         <v>7500</v>
       </c>
       <c r="E23" t="n">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="F23" t="n">
         <v>1000</v>
@@ -9774,7 +9785,7 @@
         <v>14500</v>
       </c>
       <c r="E24" t="n">
-        <v>13500</v>
+        <v>14500</v>
       </c>
       <c r="F24" t="n">
         <v>5000</v>
@@ -9816,7 +9827,7 @@
         <v>86000</v>
       </c>
       <c r="E25" t="n">
-        <v>50000</v>
+        <v>86000</v>
       </c>
       <c r="F25" t="n">
         <v>25000</v>
@@ -9858,7 +9869,7 @@
         <v>15000</v>
       </c>
       <c r="E26" t="n">
-        <v>8000</v>
+        <v>15000</v>
       </c>
       <c r="F26" t="n">
         <v>4000</v>
@@ -9937,7 +9948,7 @@
         <v>30000</v>
       </c>
       <c r="E28" t="n">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="F28" t="n">
         <v>5000</v>
@@ -9979,7 +9990,7 @@
         <v>20000</v>
       </c>
       <c r="E29" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="F29" t="n">
         <v>5000</v>
@@ -10021,7 +10032,7 @@
         <v>115000</v>
       </c>
       <c r="E30" t="n">
-        <v>50000</v>
+        <v>115000</v>
       </c>
       <c r="F30" t="n">
         <v>10000</v>
@@ -10063,7 +10074,7 @@
         <v>1500</v>
       </c>
       <c r="E31" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F31" t="n">
         <v>500</v>
@@ -10105,7 +10116,7 @@
         <v>3600</v>
       </c>
       <c r="E32" t="n">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="F32" t="n">
         <v>500</v>
@@ -10147,7 +10158,7 @@
         <v>3000</v>
       </c>
       <c r="E33" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="F33" t="n">
         <v>500</v>
@@ -10189,7 +10200,7 @@
         <v>30000</v>
       </c>
       <c r="E34" t="n">
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="F34" t="n">
         <v>5000</v>
@@ -10231,7 +10242,7 @@
         <v>3000</v>
       </c>
       <c r="E35" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="F35" t="n">
         <v>500</v>
@@ -11411,7 +11422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11452,12 +11463,17 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 6</t>
+          <t>Max Wait Product (H)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
         </is>
       </c>
     </row>
@@ -11476,18 +11492,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>5000</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
+      <c r="G2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -11513,6 +11527,9 @@
       <c r="F3" t="n">
         <v>5000</v>
       </c>
+      <c r="G3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -11537,6 +11554,9 @@
       <c r="F4" t="n">
         <v>5000</v>
       </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -11560,6 +11580,9 @@
       </c>
       <c r="F5" t="n">
         <v>5000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -11637,7 +11660,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>1.5</v>
@@ -11713,7 +11736,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D7" t="n">
         <v>1.5</v>
@@ -11732,7 +11755,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D8" t="n">
         <v>1.5</v>
@@ -11751,7 +11774,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D9" t="n">
         <v>1.5</v>
@@ -11809,7 +11832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11908,6 +11931,16 @@
           <t>Route 17</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Route 18</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Route 19</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -11982,20 +12015,30 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
@@ -12047,15 +12090,21 @@
         <v>2.03</v>
       </c>
       <c r="O3" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="Q3" t="n">
         <v>3.01</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>3.02</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>4.01</v>
       </c>
-      <c r="R3" t="n">
+      <c r="T3" t="n">
         <v>4.02</v>
       </c>
     </row>
@@ -12132,20 +12181,30 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>Devonport</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Devonport</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
@@ -12224,20 +12283,30 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
           <t>CL</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>CL</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>GBFS</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>GBFS</t>
         </is>
@@ -12316,20 +12385,30 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
           <t>CL_STORE</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>CL_STORE</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>GBFS_STORE</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>GBFS_STORE</t>
         </is>
@@ -12442,30 +12521,40 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>Newcastle</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Osborne</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Bulwer Island</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>Port Kembla</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>Bulwer Island</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>Port Kembla</t>
         </is>
@@ -12544,20 +12633,30 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
           <t>CL</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>CL</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>GBFS</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>GBFS</t>
         </is>
@@ -12636,20 +12735,30 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
           <t>CL_STORE_I</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>CL_STORE_I</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>GBFS_STORE</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>GBFS_STORE</t>
         </is>
@@ -12699,7 +12808,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Product 3 Load </t>
+          <t>Product 3 Load</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -12716,210 +12825,258 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Product 3 Load </t>
+          <t>Product 3 Store</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Product 3 Store</t>
+          <t>Destination 3 Location</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Osborne</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Osborne</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>GP_STORE</t>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Osborne</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Osborne</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Destination 3 Location</t>
+          <t>Destination 3 Unload</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Osborne</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Osborne</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Destination 3 Unload</t>
+          <t>Destination 3 Store</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>SG_STORE</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>FA_STORE</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>FA_STORE</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>FA_STORE</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Destination 3 Store</t>
+          <t>Return Location</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Gladstone</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Gladstone</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Gladstone</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>Gladstone</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>FA_STORE</t>
+          <t>Gladstone</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>FA_STORE</t>
+          <t>Gladstone</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Gladstone</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Gladstone</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>FA_STORE</t>
+          <t>Gladstone</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>GP_STORE</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Return Location</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
           <t>Gladstone</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Gladstone</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>Devonport</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>Devonport</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>Devonport</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Devonport</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Devonport</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="R20" t="inlineStr">
         <is>
           <t>Import_CL</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>Import_GBFS</t>
         </is>
@@ -13206,13 +13363,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DC6FC7C-1994-44A7-AA0F-898DA6400CD6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D234E4-8FBF-4421-B208-B98B514427EF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59B8D19-A9B5-437D-80A7-2944FB576E20}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A8FDA1F-37FD-49A0-BF48-34D5610837D7}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A637863A-3589-400E-BB0A-670CE245113A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FC3CFE4-7E91-43B1-ABC8-FE3F8171B136}"/>
 </file>
</xml_diff>

<commit_message>
Shipping Review in Progress - Codebase optimises by LLM to improve performance.
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7628,7 +7628,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:05</t>
+          <t>2025-12-21 00:27:46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7645,7 +7645,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7679,7 +7679,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7696,7 +7696,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7713,7 +7713,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7730,7 +7730,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7747,7 +7747,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7764,7 +7764,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7781,7 +7781,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:06</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7798,7 +7798,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7815,7 +7815,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7832,7 +7832,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7849,7 +7849,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7866,7 +7866,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7883,7 +7883,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7900,7 +7900,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7917,7 +7917,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7934,7 +7934,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7951,7 +7951,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7968,7 +7968,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7985,7 +7985,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -8002,7 +8002,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:07</t>
+          <t>2025-12-21 00:27:47</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8019,7 +8019,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:08</t>
+          <t>2025-12-21 00:27:48</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8036,7 +8036,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:09</t>
+          <t>2025-12-21 00:27:48</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8053,7 +8053,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:09</t>
+          <t>2025-12-21 00:27:49</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8070,7 +8070,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:10</t>
+          <t>2025-12-21 00:27:49</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8087,7 +8087,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:10</t>
+          <t>2025-12-21 00:27:50</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8104,7 +8104,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:11</t>
+          <t>2025-12-21 00:27:50</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8121,7 +8121,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:11</t>
+          <t>2025-12-21 00:27:51</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8138,7 +8138,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:12</t>
+          <t>2025-12-21 00:27:51</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8155,7 +8155,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-20 23:22:12</t>
+          <t>2025-12-21 00:27:52</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -13363,13 +13363,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D234E4-8FBF-4421-B208-B98B514427EF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEC0053-B5A3-4713-902C-EE88E0FC5925}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A8FDA1F-37FD-49A0-BF48-34D5610837D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA6EBF0B-52E0-46AA-AC42-FBC7EDC04063}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FC3CFE4-7E91-43B1-ABC8-FE3F8171B136}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89D3FFB4-7651-4ADA-A78F-91C817760B46}"/>
 </file>
</xml_diff>

<commit_message>
Shipping Logic still in progress - Slow Grind
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S109"/>
+  <dimension ref="A1:S110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,6 +686,10 @@
           <t>GladstoneStoreCL</t>
         </is>
       </c>
+      <c r="S3">
+        <f>IF(ISNA(XLOOKUP(P3,$P$2:P2,$A$2:A2)),IF(COUNTIFS($P$2:P3,P3)=1,IF(COUNTIFS($C$2:C2,C3)=0,1,MAXIFS($A$2:A2,$C$2:C2,C3)+1),A2),XLOOKUP(P3,$P$2:P2,$A$2:A2))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -5920,41 +5924,36 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
+          <t>GBFS_SUPPLY</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Make</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Port Kembla</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
           <t>GBFS_STORE</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Make</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>Port Kembla</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>VRM</t>
-        </is>
-      </c>
       <c r="K82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -5973,41 +5972,41 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
+          <t>GBFS_STORE</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Make</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Port Kembla</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
           <t>VRM</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Make</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>Port Kembla</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>SG_STORE</t>
-        </is>
-      </c>
       <c r="K83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -6026,41 +6025,41 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
+          <t>VRM</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Make</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Port Kembla</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
           <t>SG_STORE</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>Port Kembla</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -6079,31 +6078,46 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Port Kembla</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
           <t>TRUCK</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
       <c r="K85" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -6117,7 +6131,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -6127,7 +6141,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -6135,28 +6149,13 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Move</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>Port Kembla</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>SHIP</t>
-        </is>
-      </c>
       <c r="K86" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -6200,7 +6199,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>TRAIN</t>
+          <t>SHIP</t>
         </is>
       </c>
       <c r="K87" t="n">
@@ -6223,7 +6222,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>SHIP</t>
+          <t>SG_STORE</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -6233,36 +6232,36 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
           <t>Move</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Port Kembla</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRAIN</t>
         </is>
       </c>
       <c r="K88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -6276,7 +6275,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>TRAIN</t>
+          <t>SHIP</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -6301,7 +6300,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>Clyde</t>
+          <t>Melbourne</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -6315,7 +6314,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -6354,7 +6353,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>Chullora</t>
+          <t>Clyde</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -6368,7 +6367,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -6407,7 +6406,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Chullora</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -6421,7 +6420,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -6430,46 +6429,46 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Bulwer Island</t>
+          <t>Port Kembla</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>GBFS_STORE</t>
+          <t>TRAIN</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>GBFS</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
+          <t>Move</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
           <t>Store</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Make</t>
-        </is>
-      </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>Bulwer Island</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>CM10</t>
+          <t>SG_STORE</t>
         </is>
       </c>
       <c r="K92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -6518,7 +6517,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>CM11</t>
+          <t>CM10</t>
         </is>
       </c>
       <c r="K93" t="n">
@@ -6527,55 +6526,55 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
+        <v>1</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Bulwer Island</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>GBFS_STORE</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Make</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Bulwer Island</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>CM11</t>
+        </is>
+      </c>
+      <c r="K94" t="n">
         <v>2</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Bulwer Island</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>CM10</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>Make</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>Bulwer Island</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>SG_STORE</t>
-        </is>
-      </c>
-      <c r="K94" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -6594,7 +6593,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>CM11</t>
+          <t>CM10</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -6633,7 +6632,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -6647,41 +6646,41 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
+          <t>CM11</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Make</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Bulwer Island</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
           <t>SG_STORE</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Store</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Move</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>Bulwer Island</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>TRAIN</t>
-        </is>
-      </c>
       <c r="K96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -6720,7 +6719,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Deliver</t>
+          <t>Move</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -6730,7 +6729,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>TRUCK</t>
+          <t>TRAIN</t>
         </is>
       </c>
       <c r="K97" t="n">
@@ -6739,7 +6738,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -6753,7 +6752,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>TRAIN</t>
+          <t>SG_STORE</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -6763,7 +6762,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Move</t>
+          <t>Store</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -6773,21 +6772,21 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>Tennyson</t>
+          <t>Bulwer Island</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="K98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -6806,7 +6805,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>TRUCK</t>
+          <t>TRAIN</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -6816,7 +6815,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Deliver</t>
+          <t>Move</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -6824,13 +6823,28 @@
           <t>SG</t>
         </is>
       </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Tennyson</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
       <c r="K99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -6839,12 +6853,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Tennyson</t>
+          <t>Bulwer Island</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -6854,7 +6868,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -6862,66 +6876,66 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>Tennyson</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K100" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
+        <v>1</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Tennyson</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Tennyson</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>TRUCK</t>
+        </is>
+      </c>
+      <c r="K101" t="n">
         <v>2</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Tennyson</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="K101" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -6930,12 +6944,12 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Tennyson</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -6945,7 +6959,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -6953,28 +6967,13 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>Melbourne</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K102" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -6988,31 +6987,46 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
           <t>TRUCK</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
       <c r="K103" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -7021,12 +7035,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Clyde</t>
+          <t>Melbourne</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -7036,7 +7050,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -7044,28 +7058,13 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>Clyde</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K104" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -7079,31 +7078,46 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Clyde</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
           <t>TRUCK</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
       <c r="K105" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -7112,12 +7126,12 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Chullora</t>
+          <t>Clyde</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -7127,7 +7141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -7135,28 +7149,13 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>Chullora</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K106" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -7170,31 +7169,46 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Chullora</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
           <t>TRUCK</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
       <c r="K107" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -7203,12 +7217,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Chullora</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>SG_STORE</t>
+          <t>TRUCK</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -7218,7 +7232,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>Deliver</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -7226,60 +7240,98 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>Deliver</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>Newcastle</t>
-        </is>
-      </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>TRUCK</t>
-        </is>
-      </c>
       <c r="K108" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
+        <v>1</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>SG_STORE</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>TRUCK</t>
+        </is>
+      </c>
+      <c r="K109" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
         <v>2</v>
       </c>
-      <c r="B109" t="inlineStr">
+      <c r="B110" t="inlineStr">
         <is>
           <t>SG</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="C110" t="inlineStr">
         <is>
           <t>Newcastle</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
+      <c r="D110" t="inlineStr">
         <is>
           <t>TRUCK</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E110" t="inlineStr">
         <is>
           <t>SG</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
+      <c r="F110" t="inlineStr">
         <is>
           <t>Deliver</t>
         </is>
       </c>
-      <c r="G109" t="inlineStr">
+      <c r="G110" t="inlineStr">
         <is>
           <t>SG</t>
         </is>
       </c>
-      <c r="K109" t="n">
+      <c r="K110" t="n">
         <v>4</v>
       </c>
     </row>
@@ -7628,7 +7680,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7645,7 +7697,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7655,14 +7707,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>rows=108 from Model Inputs.xlsx</t>
+          <t>rows=109 from Model Inputs.xlsx</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7679,7 +7731,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7689,14 +7741,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Make -&gt; Make, rows=13</t>
+          <t>Make -&gt; Make, rows=14</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7713,7 +7765,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7730,7 +7782,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7747,7 +7799,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7764,7 +7816,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7781,7 +7833,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7798,7 +7850,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7815,7 +7867,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7832,7 +7884,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7849,7 +7901,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7859,14 +7911,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Network rows=108 -&gt; generated_model_inputs.xlsx</t>
+          <t>Network rows=109 -&gt; generated_model_inputs.xlsx</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7883,7 +7935,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -7893,14 +7945,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Make rows=13 -&gt; generated_model_inputs.xlsx</t>
+          <t>Make rows=14 -&gt; generated_model_inputs.xlsx</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -7917,7 +7969,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7934,7 +7986,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7951,7 +8003,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7968,7 +8020,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7985,7 +8037,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -8002,7 +8054,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:19</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8019,7 +8071,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:20</t>
+          <t>2025-12-22 18:20:05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8036,7 +8088,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:20</t>
+          <t>2025-12-22 18:20:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8053,7 +8105,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:20</t>
+          <t>2025-12-22 18:20:06</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8070,7 +8122,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:21</t>
+          <t>2025-12-22 18:20:07</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8087,7 +8139,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:21</t>
+          <t>2025-12-22 18:20:07</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8104,7 +8156,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:22</t>
+          <t>2025-12-22 18:20:07</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8121,7 +8173,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:22</t>
+          <t>2025-12-22 18:20:08</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8138,7 +8190,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:22</t>
+          <t>2025-12-22 18:20:08</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8155,7 +8207,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-21 22:48:23</t>
+          <t>2025-12-22 18:20:08</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -8243,7 +8295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8593,35 +8645,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>VRM</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>CL</t>
+          <t>GBFS_SUPPLY</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>GBFS</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>205</v>
+        <v>60</v>
       </c>
       <c r="F10" t="n">
         <v>10</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1-5,53,96-100,148,191,234,277,320,363</t>
-        </is>
-      </c>
       <c r="H10" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -8637,16 +8679,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GBFS</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="F11" t="n">
         <v>10</v>
@@ -8660,41 +8702,46 @@
         <v>0.05</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Railton</t>
+          <t>Port Kembla</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CM4</t>
+          <t>VRM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>GBFS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1-5,53,96-100,148,191,234,277,320,363</t>
+        </is>
+      </c>
       <c r="H12" t="n">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="I12" t="n">
-        <v>0.88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -8705,7 +8752,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CM5</t>
+          <t>CM4</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -8719,7 +8766,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="F13" t="n">
         <v>10</v>
@@ -8739,29 +8786,63 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>CM5</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F14" t="n">
         <v>10</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Railton</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>150</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>95-120</t>
         </is>
       </c>
-      <c r="H14" t="n">
+      <c r="H15" t="n">
         <v>0.0298</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11422,7 +11503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11463,17 +11544,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Max Wait Product (H)</t>
+          <t>Unnamed: 6</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 7</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 8</t>
         </is>
       </c>
     </row>
@@ -11495,14 +11571,11 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>5000</v>
       </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -11527,9 +11600,6 @@
       <c r="F3" t="n">
         <v>5000</v>
       </c>
-      <c r="G3" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -11554,9 +11624,6 @@
       <c r="F4" t="n">
         <v>5000</v>
       </c>
-      <c r="G4" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -11580,9 +11647,6 @@
       </c>
       <c r="F5" t="n">
         <v>5000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -12880,6 +12944,11 @@
           <t>Osborne</t>
         </is>
       </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr">
         <is>
           <t>Osborne</t>
@@ -12927,6 +12996,11 @@
           <t>GP</t>
         </is>
       </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr">
         <is>
           <t>GP</t>
@@ -12970,6 +13044,11 @@
         </is>
       </c>
       <c r="N19" t="inlineStr">
+        <is>
+          <t>GP_STORE</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>GP_STORE</t>
         </is>
@@ -13363,13 +13442,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86E108E9-B29B-4582-8C6F-4CC86BF8FC08}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE88CA25-650E-4CBF-8073-FE67886C22D1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD7BD9-389A-4610-B026-07B578585B87}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B668DA8E-A63B-4CE9-AA0F-6644AC06AF7A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85AD61D-5DBF-446B-9BC8-8597F1388D1B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1A007E-160E-4DA0-BF92-507C4367F757}"/>
 </file>
</xml_diff>

<commit_message>
Shipping Logic still in progress - Slow Grind - 24 Dec 2025
</commit_message>
<xml_diff>
--- a/generated_model_inputs.xlsx
+++ b/generated_model_inputs.xlsx
@@ -7733,7 +7733,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7750,7 +7750,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7767,7 +7767,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7777,14 +7777,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Settings -&gt; Settings, rows=3</t>
+          <t>Settings -&gt; Settings, rows=25</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7818,7 +7818,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7835,7 +7835,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7852,7 +7852,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7869,7 +7869,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:58</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7886,7 +7886,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7903,7 +7903,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7920,7 +7920,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -7937,7 +7937,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -7954,7 +7954,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -7971,7 +7971,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -7981,14 +7981,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Settings rows=3 -&gt; generated_model_inputs.xlsx</t>
+          <t>Settings rows=25 -&gt; generated_model_inputs.xlsx</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -8005,7 +8005,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -8022,7 +8022,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:16</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -8039,7 +8039,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -8056,7 +8056,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -8073,7 +8073,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -8090,7 +8090,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -8107,7 +8107,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -8124,7 +8124,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:54:59</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -8134,14 +8134,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>added=0, updated=0</t>
+          <t>added=16, updated=0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:17</t>
+          <t>2025-12-23 22:55:00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -8158,7 +8158,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:18</t>
+          <t>2025-12-23 22:55:00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -8175,7 +8175,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:18</t>
+          <t>2025-12-23 22:55:00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -8192,7 +8192,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:18</t>
+          <t>2025-12-23 22:55:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -8209,7 +8209,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:19</t>
+          <t>2025-12-23 22:55:01</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -8226,7 +8226,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:19</t>
+          <t>2025-12-23 22:55:01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -8243,7 +8243,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:20</t>
+          <t>2025-12-23 22:55:02</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8260,7 +8260,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-23 01:13:20</t>
+          <t>2025-12-23 22:55:02</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -8285,7 +8285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8308,32 +8308,161 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Number of Simulation Runs</t>
+          <t>horizon_days</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>500</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Modeling Horizon (#Days)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>365</v>
+          <t>random_opening</t>
+        </is>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Time Buckets (Days, Half Days, Hours)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hours</t>
+          <t>random_seed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>progress_step_pct</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>demand_truck_load_tons</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>demand_step_hours</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>require_full_payload</t>
+        </is>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ship_idle_wait_h</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ship_max_wait_product_h</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>transporter_wait_h</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mean_breakdown_duration</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>make_output_choice</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>min_fill_pct</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>step_hours</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>write_plots</t>
+        </is>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>write_csvs</t>
+        </is>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>out_dir</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sim_outputs</t>
         </is>
       </c>
     </row>
@@ -13571,13 +13700,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B9952CE-D806-49A4-AC83-FEDCE4676CCC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9DDE614-C431-4356-B2CF-405FB7706216}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16EE422-F531-4CE9-8305-F45FF25EAF33}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B98720-84ED-4915-9928-A656149833BB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024E2D85-74D3-4B09-8C89-CB9DB88D5F78}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F8DB1D4-13A9-44FC-85EB-3EFB914C08C5}"/>
 </file>
</xml_diff>